<commit_message>
feat: add watermark to test DBC credetnial
Signed-off-by: Akiff Manji <amanji@petridish.dev>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/bcgov-digital-trust/business-card/OCA.xlsx
+++ b/OCABundles/schema/bcgov-digital-trust/business-card/OCA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanji/projects/aries-oca-bundles/OCABundles/schema/bcgov-digital-trust/business-card/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanji/projects/bcgov/aries-oca-bundles/OCABundles/schema/bcgov-digital-trust/business-card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDE8F97-A12E-8C4A-91DD-8EFA9ABED267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A050C8D8-948A-174C-9019-E411AA8D8B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2145,7 +2145,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2343,6 +2343,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2384,9 +2390,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -2394,6 +2397,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+        <name val="Helvetica Neue"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2465,12 +2480,58 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF16E7CF"/>
+        <name val="Helvetica Neue"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEF2CB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+        <name val="Helvetica Neue"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
         <name val="Helvetica Neue"/>
         <charset val="1"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFECECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF16E7CF"/>
+        <name val="Helvetica Neue"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEF2CB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2494,29 +2555,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFECECEC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-        <name val="Helvetica Neue"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFFBE4D5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2534,30 +2573,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
-        <name val="Helvetica Neue"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFECECEC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF16E7CF"/>
-        <name val="Helvetica Neue"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF00B050"/>
         <name val="Helvetica Neue"/>
         <charset val="1"/>
@@ -2565,18 +2580,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF16E7CF"/>
-        <name val="Helvetica Neue"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEF2CB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3099,28 +3102,28 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="78"/>
     </row>
     <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
@@ -3140,10 +3143,10 @@
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="77"/>
+      <c r="D8" s="79"/>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="B9" s="7"/>
@@ -3159,33 +3162,33 @@
       <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="71"/>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3241,11 +3244,11 @@
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
     </row>
     <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.15">
       <c r="B4" s="2"/>
@@ -3264,7 +3267,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="80" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -3275,7 +3278,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B7" s="82"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="19" t="s">
         <v>17</v>
       </c>
@@ -3284,7 +3287,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B8" s="82"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="19" t="s">
         <v>19</v>
       </c>
@@ -3293,7 +3296,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B9" s="82"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="19" t="s">
         <v>21</v>
       </c>
@@ -3335,7 +3338,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="64" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="85" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -3346,7 +3349,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B14" s="83"/>
+      <c r="B14" s="85"/>
       <c r="C14" s="19" t="s">
         <v>35</v>
       </c>
@@ -3388,7 +3391,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="85" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -3399,7 +3402,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B19" s="83"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="19" t="s">
         <v>49</v>
       </c>
@@ -3441,7 +3444,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="85" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="21"/>
@@ -3450,7 +3453,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B24" s="83"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="19" t="s">
         <v>62</v>
       </c>
@@ -3459,7 +3462,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B25" s="83"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="19" t="s">
         <v>64</v>
       </c>
@@ -3468,7 +3471,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B26" s="83"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="19" t="s">
         <v>66</v>
       </c>
@@ -3477,7 +3480,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B27" s="83"/>
+      <c r="B27" s="85"/>
       <c r="C27" s="19" t="s">
         <v>68</v>
       </c>
@@ -3486,7 +3489,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="96" x14ac:dyDescent="0.15">
-      <c r="B28" s="83"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="19" t="s">
         <v>70</v>
       </c>
@@ -3495,7 +3498,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B29" s="83"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="19" t="s">
         <v>72</v>
       </c>
@@ -3504,7 +3507,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B30" s="83"/>
+      <c r="B30" s="85"/>
       <c r="C30" s="19" t="s">
         <v>74</v>
       </c>
@@ -3536,18 +3539,18 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
     </row>
     <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
     </row>
     <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="25" t="s">
@@ -3611,16 +3614,16 @@
       <c r="D44" s="32"/>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="72"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4597,11 +4600,11 @@
     <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="NOT NEEDED">
       <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="27" operator="containsText" text="OPTIONAL">
+    <cfRule type="containsText" dxfId="15" priority="28" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="27" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH("OPTIONAL",C18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="28" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH("REQUIRED",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C32 C6">
@@ -4610,36 +4613,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="12" priority="54" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C31)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="56" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C31)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="11" priority="55" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH("OPTIONAL",C31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="56" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH("REQUIRED",C31)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="54" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C984">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C47)))</formula>
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="REQUIRED">
+      <formula>NOT(ISERROR(SEARCH("REQUIRED",C47)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH("OPTIONAL",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="REQUIRED">
-      <formula>NOT(ISERROR(SEARCH("REQUIRED",C47)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F28 C10:C17 C32:C33">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="NOT NEEDED">
-      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="OPTIONAL">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="OPTIONAL">
       <formula>NOT(ISERROR(SEARCH("OPTIONAL",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="REQUIRED">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="REQUIRED">
       <formula>NOT(ISERROR(SEARCH("REQUIRED",C6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="NOT NEEDED">
+      <formula>NOT(ISERROR(SEARCH("NOT NEEDED",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -36884,7 +36887,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -36972,7 +36975,7 @@
       <c r="A5" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="69" t="s">
         <v>144</v>
       </c>
       <c r="C5" s="47" t="str">
@@ -37011,7 +37014,7 @@
       <c r="A6" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="69" t="s">
         <v>143</v>
       </c>
       <c r="C6" s="47" t="str">
@@ -37195,8 +37198,8 @@
       <c r="Z10" s="26"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="47" t="str">
         <f>IF(ISBLANK(Main!$B11),"",Main!$B11)</f>
         <v>family_name</v>
@@ -67995,7 +67998,7 @@
       <formula>AND(NOT(ISBLANK(D4)),$C4="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" sqref="D4:D1003" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$D$4:$D$1003</formula1>
       <formula2>0</formula2>

</xml_diff>